<commit_message>
Update BSides19 Project Summary.xlsx
updating Values in Project Summary
</commit_message>
<xml_diff>
--- a/admin docs/BSides19 Project Summary.xlsx
+++ b/admin docs/BSides19 Project Summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="528" documentId="11_F25DC773A252ABEACE02EC2C3B9B477C5ADE5898" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{D419C4A3-CDC4-40EE-B2F4-FB8234CC6052}"/>
+  <xr:revisionPtr revIDLastSave="559" documentId="11_F25DC773A252ABEACE02EC2C3B9B477C5ADE5898" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9D4D8A4F-9660-4BE8-A181-F9E4C4FA71CC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Summary" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
   <si>
     <t>https://www.mouser.com/ProductDetail/Espressif-Systems/ESP-WROOM-02D?qs=sGAEpiMZZMve4%2fbfQkoj%252bFo2lZdnZgOU6INDYnTf7ns%3d</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Code info</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>BOM Complete (Y/N)</t>
   </si>
   <si>
@@ -343,6 +340,15 @@
   </si>
   <si>
     <t>Project Name</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Customer Supplied</t>
+  </si>
+  <si>
+    <t>Kids Badge</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,8 +426,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,8 +488,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -921,6 +941,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -929,7 +986,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1075,10 +1132,24 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -1363,242 +1434,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E24C87-6631-4852-AEA5-9113B088B520}">
-  <dimension ref="B2:H28"/>
+  <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="87" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C2" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="86" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C3" s="90" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="92"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="5">
         <v>3500</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="86">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="83">
         <v>43417</v>
       </c>
-      <c r="D5" s="86"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="85">
+      <c r="D5" s="83"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="84">
         <v>43556</v>
       </c>
-      <c r="D6" s="85"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="84">
+      <c r="D6" s="84"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="89">
         <f>SUM(C11,D11,E11,F11,G11,H11)</f>
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="86" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="86" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G10" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="83">
+      <c r="I10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="85">
         <v>150</v>
       </c>
-      <c r="D11" s="83">
+      <c r="D11" s="85">
         <v>350</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="85">
         <v>25</v>
       </c>
-      <c r="F11" s="83">
+      <c r="F11" s="85">
         <v>15</v>
       </c>
-      <c r="G11" s="83">
+      <c r="G11" s="85">
         <v>10</v>
       </c>
-      <c r="H11" s="83">
+      <c r="H11" s="85">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="I11" s="4">
+        <v>50</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="I12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="86" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="86" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="86" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="86" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C18">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="86" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="C28" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="333" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1618,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230ECA56-04B2-4271-9B6D-69C62BBA135C}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates of Images and Gerbers
Adding new Images and Gerbers to Boards
</commit_message>
<xml_diff>
--- a/admin docs/BSides19 Project Summary.xlsx
+++ b/admin docs/BSides19 Project Summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="64" documentId="6_{1FF347B4-B7B3-494A-B430-3C9EE18135A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{187A9831-FE31-49C7-B6B7-829D6E19AC2D}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="6_{1FF347B4-B7B3-494A-B430-3C9EE18135A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{EEBC519E-BC04-4E81-91E0-BE6268BC3ABE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Summary" sheetId="5" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Con Badge AP</t>
   </si>
   <si>
-    <t>Battery Holders 2x AA</t>
-  </si>
-  <si>
     <t>Kids Badge AP</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/75-XFree-shipping-2032-CR2032-3v-220mAh-lithium-Button-Coin-Battery-in-Bulk-for-watches-toys/32725154601.html?spm=2114.search0104.3.92.347522566EsRWR&amp;ws_ab_test=searchweb0_0,searchweb201602_3_10065_10068_10130_10890_10547_319_10546_317_5730318_10548_5729218_10545_10696_453_10084_454_10083_10618_10307_538_537_536_10059_10884_10887_100031_321_322_10103,searchweb201603_51,ppcSwitch_0&amp;algo_expid=92bb5bac-c7f3-4ead-96d8-d84fe5f17d5a-13&amp;algo_pvid=92bb5bac-c7f3-4ead-96d8-d84fe5f17d5a</t>
+  </si>
+  <si>
+    <t>Battery Holders 2x AAA</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1066,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1203,6 +1203,8 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1236,7 +1238,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -1273,8 +1274,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>109147</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -1293,7 +1294,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -1338,8 +1339,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>110227</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -1358,7 +1359,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -1733,37 +1734,37 @@
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B2" s="80" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
+      <c r="C2" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
+      <c r="C3" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="5">
         <v>3500</v>
@@ -1778,7 +1779,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="76">
         <v>43417</v>
@@ -1793,7 +1794,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="77">
         <v>43556</v>
@@ -1808,7 +1809,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="81">
         <f>SUM(C11,D11,E11,F11,G11,H11)</f>
@@ -1824,10 +1825,10 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1839,10 +1840,10 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1854,34 +1855,34 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="I10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="78">
         <v>150</v>
@@ -1908,91 +1909,91 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2004,61 +2005,61 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -2079,13 +2080,13 @@
         <v>1</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" s="79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2098,7 +2099,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2111,10 +2112,10 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2122,13 +2123,13 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2141,7 +2142,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -2154,7 +2155,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2180,10 +2181,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2191,7 +2192,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J31" s="4"/>
     </row>
@@ -2221,7 +2222,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="82">
         <v>43581</v>
@@ -2229,7 +2230,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="82">
         <v>43574</v>
@@ -2237,7 +2238,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="82">
         <v>43560</v>
@@ -2245,7 +2246,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="82">
         <v>43493</v>
@@ -2253,7 +2254,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="82">
         <v>43482</v>
@@ -2261,12 +2262,12 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="82">
         <v>43475</v>
@@ -2274,7 +2275,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="83">
         <v>43456</v>
@@ -2282,7 +2283,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="82">
         <v>43474</v>
@@ -2319,34 +2320,34 @@
   <sheetData>
     <row r="1" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="95"/>
-      <c r="E2" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="95"/>
-      <c r="H2" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="95"/>
+      <c r="B2" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="E2" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="97"/>
+      <c r="H2" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="97"/>
     </row>
     <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="31">
         <v>150</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="30">
         <v>50</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="30">
         <v>100</v>
@@ -2354,7 +2355,7 @@
     </row>
     <row r="4" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="66">
         <f>C25</f>
@@ -2363,18 +2364,18 @@
     </row>
     <row r="5" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="6" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="E6" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="93"/>
-      <c r="H6" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="93"/>
+      <c r="C6" s="95"/>
+      <c r="E6" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="95"/>
+      <c r="H6" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="95"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="54" t="s">
@@ -2461,19 +2462,19 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B11" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="61">
         <v>0</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="61">
         <v>0</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="61"/>
     </row>
@@ -2546,7 +2547,7 @@
         <v>163</v>
       </c>
       <c r="K14" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L14" s="42">
         <f>C14+F14</f>
@@ -2559,21 +2560,21 @@
     </row>
     <row r="16" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="44">
         <f>C14 / (C3+C4)</f>
         <v>3.9743421052631578</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="44">
         <f>F14/F3</f>
         <v>6.49</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" s="44">
         <f>I14/I3</f>
@@ -2582,14 +2583,14 @@
     </row>
     <row r="18" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="19" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="95"/>
+      <c r="B19" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="97"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="70">
         <v>550</v>
@@ -2597,7 +2598,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="67">
         <v>25</v>
@@ -2605,7 +2606,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="67">
         <v>10</v>
@@ -2613,7 +2614,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="67">
         <v>15</v>
@@ -2621,7 +2622,7 @@
     </row>
     <row r="24" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="68">
         <v>10</v>
@@ -2636,27 +2637,27 @@
     <row r="27" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="28" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B28" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B32" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2680,7 @@
   <dimension ref="B1:K18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2697,18 +2698,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
@@ -2740,13 +2741,13 @@
         <v>150</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
       <c r="C4" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -2816,8 +2817,8 @@
         <f>I6*J3</f>
         <v>171.00000000000003</v>
       </c>
-      <c r="K6" s="99" t="s">
-        <v>122</v>
+      <c r="K6" s="88" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.45">
@@ -2971,18 +2972,18 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="98"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="100"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="25" t="s">
@@ -3094,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4301377-AA15-484C-9B9E-5F5D243282E9}">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3106,18 +3107,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
@@ -3153,7 +3154,7 @@
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
       <c r="C4" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -3179,7 +3180,7 @@
     <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3376,18 +3377,18 @@
     </row>
     <row r="13" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="98"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="100"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="25" t="s">
@@ -3497,8 +3498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18EF07E-B53E-4959-AFC9-08CFAA150A1A}">
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3510,18 +3511,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
@@ -3557,14 +3558,14 @@
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="14"/>
       <c r="C4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="5">
         <v>0.1</v>
@@ -3580,19 +3581,19 @@
         <f>I4*J3</f>
         <v>10</v>
       </c>
-      <c r="K4" s="20" t="s">
-        <v>52</v>
+      <c r="K4" s="89" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="5">
         <v>0.05</v>
@@ -3620,7 +3621,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="10">
         <v>0.01</v>
@@ -3652,18 +3653,18 @@
     </row>
     <row r="8" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="9" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="97"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="98"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="100"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="25" t="s">
@@ -3699,13 +3700,13 @@
     <row r="11" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="14"/>
       <c r="C11" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="F11" s="65">
         <v>2032</v>
@@ -3725,13 +3726,13 @@
         <v>20</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="84"/>
       <c r="C12" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -3792,7 +3793,10 @@
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B9:K9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{65DE6BE3-3471-4C52-88D0-04E394F4D3CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FG updates from Compute
Photos, Gerberts for Test
</commit_message>
<xml_diff>
--- a/admin docs/BSides19 Project Summary.xlsx
+++ b/admin docs/BSides19 Project Summary.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="68" documentId="6_{1FF347B4-B7B3-494A-B430-3C9EE18135A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{EEBC519E-BC04-4E81-91E0-BE6268BC3ABE}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="6_{1FF347B4-B7B3-494A-B430-3C9EE18135A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A93FEF17-72BE-44F1-B234-373622BD33D1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Summary" sheetId="5" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>https://www.mouser.com/ProductDetail/Espressif-Systems/ESP-WROOM-02D?qs=sGAEpiMZZMve4%2fbfQkoj%252bFo2lZdnZgOU6INDYnTf7ns%3d</t>
   </si>
   <si>
-    <t>battery Holders 2x AA</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/keystone-electronics/2462/36-2462-ND/303811</t>
   </si>
   <si>
@@ -403,6 +400,33 @@
   </si>
   <si>
     <t>Battery Holders 2x AAA</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Budget Quote</t>
+  </si>
+  <si>
+    <t>Profit %</t>
+  </si>
+  <si>
+    <t>Profit Table</t>
+  </si>
+  <si>
+    <t>Shipping Costs</t>
+  </si>
+  <si>
+    <t>Shipping Cost</t>
+  </si>
+  <si>
+    <t>battery Holders 2x AAA</t>
+  </si>
+  <si>
+    <t>AAA Battery</t>
+  </si>
+  <si>
+    <t>SMD</t>
   </si>
 </sst>
 </file>
@@ -489,7 +513,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,8 +572,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1058,15 +1094,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1198,13 +1265,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="2" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1229,6 +1316,12 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,12 +1332,13 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1391,6 +1485,266 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1086600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>125557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1102080</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>138877</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE7663CD-BD99-4801-83D3-6E4B0B5DFAC7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12945225" y="1044720"/>
+            <a:ext cx="15480" cy="13320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE7663CD-BD99-4801-83D3-6E4B0B5DFAC7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12936585" y="1035720"/>
+              <a:ext cx="33120" cy="30960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1154280</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1173720</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>98557</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{678846CD-BC3A-43D7-9EE9-EE047D2B63BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13012905" y="1014480"/>
+            <a:ext cx="19440" cy="3240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{678846CD-BC3A-43D7-9EE9-EE047D2B63BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13004265" y="1005840"/>
+              <a:ext cx="37080" cy="20880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1096320</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>113317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1108560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>116197</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7573FBF-1C0E-4E8E-8AE1-0C679F43D8E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12954945" y="1032480"/>
+            <a:ext cx="12240" cy="2880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7573FBF-1C0E-4E8E-8AE1-0C679F43D8E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12945945" y="1023840"/>
+              <a:ext cx="29880" cy="20520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1157520</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>106837</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1205040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>129877</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A04336D-B13B-4058-9D49-AE3790C232BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13016145" y="1026000"/>
+            <a:ext cx="47520" cy="23040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A04336D-B13B-4058-9D49-AE3790C232BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13007145" y="1017360"/>
+              <a:ext cx="65160" cy="40680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1453,6 +1807,130 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 77 9584 0 0,'0'0'208'0'0,"0"0"48"0"0,0 0 0 0 0,0 0 24 0 0,0 0-280 0 0,2-7 0 0 0,7 0 0 0 0,-2 2 0 0 0,-7-2 64 0 0,0 0-64 0 0,7 4 0 0 0,1-4 0 0 0,3 0 0 0 0,-4 0 0 0 0,-7 0 0 0 0,4 1-2832 0 0,7-1-584 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-01-08T02:27:17.592"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 36 9472 0 0,'0'0'432'0'0,"0"0"-6"0"0,0 0-228 0 0,0 0 64 0 0,16-6 918 0 0,1-11-724 0 0,-17 17-372 0 0,5-7 215 0 0,-2 2-342 0 0,-3 4-246 0 0,0 1-70 0 0,0 0-477 0 0,0 0-1972 0 0,0 0-842 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-01-08T02:27:18.137"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 3224 0 0,'0'0'456'0'0,"0"0"707"0"0,0 0 311 0 0,0 0 59 0 0,0 0-151 0 0,0 0-705 0 0,0 0-313 0 0,2 0-63 0 0,1 2-177 0 0,-2-2-87 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0-37 0 0,18 0-812 0 0,-19 0-2937 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-01-08T02:27:18.847"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 5984 0 0,'0'0'536'0'0,"0"0"-432"0"0,0 0-104 0 0,0 0 0 0 0,0 0 1024 0 0,0 0 176 0 0,0 0 40 0 0,0 0 8 0 0,0 0-1000 0 0,11 2-248 0 0,-11-2 0 0 0,11 0-3056 0 0,0 5-656 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-01-08T02:27:20.747"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 59 10104 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 0-271 0 0,0 0-51 0 0,0 0 11 0 0,0 0 1 0 0,0 0 8 0 0,0 0-88 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-64 0 0,19-11 471 0 0,-15 9-428 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1-1 0 0 0,2 0-43 0 0,-4 4 80 0 0,0 1 71 0 0,0 0 29 0 0,0 0 4 0 0,0 0 13 0 0,0 0 58 0 0,0 0 29 0 0,0 0 4 0 0,0 0-16 0 0,0 0-68 0 0,0 0-32 0 0,0 0-5 0 0,0 0 0 0 0,0 0-7 0 0,0 0-7 0 0,0 0-1 0 0,20-1 1502 0 0,-4-1-912 0 0,-15 2-717 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-25 0 0,-1-1-510 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1729,45 +2207,46 @@
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B2" s="80" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
+      <c r="C2" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="93"/>
+      <c r="C3" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="109"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5">
-        <v>3500</v>
+        <v>6000</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1779,7 +2258,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="76">
         <v>43417</v>
@@ -1794,7 +2273,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="77">
         <v>43556</v>
@@ -1809,7 +2288,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="81">
         <f>SUM(C11,D11,E11,F11,G11,H11)</f>
@@ -1825,10 +2304,10 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1840,10 +2319,10 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1855,40 +2334,40 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="I10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="78">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D11" s="78">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E11" s="78">
         <v>25</v>
@@ -1909,91 +2388,91 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2005,67 +2484,67 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -2080,13 +2559,13 @@
         <v>1</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" s="79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2099,7 +2578,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="79" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2112,10 +2591,10 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2123,13 +2602,13 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2142,7 +2621,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -2155,7 +2634,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2168,7 +2647,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2181,10 +2660,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2192,7 +2671,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J31" s="4"/>
     </row>
@@ -2211,18 +2690,18 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="82">
         <v>43581</v>
@@ -2230,7 +2709,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="82">
         <v>43574</v>
@@ -2238,7 +2717,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="82">
         <v>43560</v>
@@ -2246,7 +2725,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="82">
         <v>43493</v>
@@ -2254,7 +2733,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="82">
         <v>43482</v>
@@ -2262,28 +2741,28 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+      <c r="B8" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="103">
+        <v>43475</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="82">
-        <v>43475</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="83">
+      <c r="C9" s="101">
         <v>43456</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="82">
         <v>43474</v>
@@ -2296,379 +2775,456 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230ECA56-04B2-4271-9B6D-69C62BBA135C}">
-  <dimension ref="B1:L32"/>
+  <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.53125" customWidth="1"/>
+    <col min="2" max="2" width="27.53125" customWidth="1"/>
+    <col min="3" max="3" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1328125" customWidth="1"/>
-    <col min="5" max="5" width="23.265625" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="5.73046875" customWidth="1"/>
-    <col min="8" max="8" width="24.265625" customWidth="1"/>
+    <col min="7" max="7" width="5.796875" customWidth="1"/>
+    <col min="8" max="8" width="24.19921875" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="3.86328125" customWidth="1"/>
-    <col min="11" max="11" width="11.59765625" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.53125" customWidth="1"/>
+    <col min="12" max="12" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1328125" customWidth="1"/>
+    <col min="16" max="16" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="96" t="s">
+    <row r="1" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="112" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="113"/>
+      <c r="E2" s="112" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="113"/>
+      <c r="H2" s="112" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="113"/>
+    </row>
+    <row r="3" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="E2" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="97"/>
-      <c r="H2" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="97"/>
-    </row>
-    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="75" t="s">
-        <v>61</v>
-      </c>
       <c r="C3" s="31">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="30">
         <v>50</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" s="30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="66">
-        <f>C25</f>
-        <v>610</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="94" t="s">
+        <f>C26</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="110" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="111"/>
+      <c r="E6" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="E6" s="94" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="95"/>
-      <c r="H6" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="95"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F6" s="111"/>
+      <c r="H6" s="110" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="111"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B7" s="54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="58">
         <v>400</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="58">
         <v>0</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="58">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B8" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="59">
         <v>425</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="59">
         <v>0</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="59">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B9" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="60">
-        <f>'ConBadge BOM'!J12</f>
-        <v>790.5</v>
+        <f>'ConBadge BOM'!J11</f>
+        <v>1112.5</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="60">
         <f>'KidsBadge BOM'!J12</f>
         <v>173.5</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="60">
         <f>'LTS BOM'!J7</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B10" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="71">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="71">
         <v>26</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="71">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B11" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="61">
-        <v>0</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C11" s="61"/>
       <c r="E11" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="61">
-        <v>0</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F11" s="61"/>
       <c r="H11" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="61"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B12" s="55" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="C12" s="61">
+        <v>100</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="61"/>
+      <c r="H12" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="61"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B13" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="61">
         <f>(C3+C4)*1.5</f>
-        <v>1140</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="61">
+        <v>1215</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="61">
         <f>(F3)*1.5</f>
         <v>75</v>
       </c>
-      <c r="H12" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="61">
-        <f>(I3)*0.8</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="62">
+      <c r="H13" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="61">
+        <f>I3*1</f>
+        <v>150</v>
+      </c>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="95"/>
+    </row>
+    <row r="14" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="62">
         <f>'ConBadge BOM'!J18</f>
-        <v>213</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="62">
+        <v>505</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="62">
         <f>'KidsBadge BOM'!J18</f>
         <v>50</v>
       </c>
-      <c r="H13" s="56" t="s">
+      <c r="H14" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="62">
+        <f>'LTS BOM'!J14</f>
+        <v>61.5</v>
+      </c>
+      <c r="O14" s="96"/>
+      <c r="P14" s="97"/>
+      <c r="Q14" s="95"/>
+    </row>
+    <row r="15" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="62">
-        <f>'LTS BOM'!J14</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="63">
-        <f>SUM(C7:C13)</f>
-        <v>3020.5</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="63">
-        <f>SUM(F7:F13)</f>
+      <c r="C15" s="63">
+        <f>SUM(C7:C14)</f>
+        <v>3907.5</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="63">
+        <f>SUM(F7:F14)</f>
         <v>324.5</v>
       </c>
-      <c r="H14" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="63">
-        <f>SUM(I7:I13)</f>
-        <v>163</v>
-      </c>
-      <c r="K14" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" s="42">
-        <f>C14+F14</f>
-        <v>3345</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="41" t="s">
+      <c r="H15" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="63">
+        <f>SUM(I7:I14)</f>
+        <v>261.5</v>
+      </c>
+      <c r="K15" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="44">
-        <f>C14 / (C3+C4)</f>
-        <v>3.9743421052631578</v>
-      </c>
-      <c r="E16" s="41" t="s">
+      <c r="L15" s="42">
+        <f>C15+F15</f>
+        <v>4232</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="97"/>
+      <c r="Q15" s="95"/>
+    </row>
+    <row r="16" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="95"/>
+    </row>
+    <row r="17" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="44">
+        <f>C15 / (C3+C4)</f>
+        <v>4.8240740740740744</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="44">
+        <f>F15/F3</f>
+        <v>6.49</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="44">
+        <f>I15/I3</f>
+        <v>1.7433333333333334</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="100"/>
+      <c r="Q17" s="95"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="L18" s="3"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="95"/>
+    </row>
+    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+    </row>
+    <row r="20" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="112" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="113"/>
+      <c r="H20" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="115"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B21" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="70">
+        <v>500</v>
+      </c>
+      <c r="H21" s="92" t="s">
+        <v>124</v>
+      </c>
+      <c r="I21" s="89">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B22" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="67">
+        <v>25</v>
+      </c>
+      <c r="H22" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="44">
-        <f>F14/F3</f>
-        <v>6.49</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="44">
-        <f>I14/I3</f>
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="19" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="96" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="97"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="70">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="73" t="s">
+      <c r="I22" s="90">
+        <f>L15</f>
+        <v>4232</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B23" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="67">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="73" t="s">
+      <c r="C23" s="67">
+        <v>10</v>
+      </c>
+      <c r="H23" s="93" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="90">
+        <f>I21-I22</f>
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="67">
+      <c r="C24" s="67">
+        <v>15</v>
+      </c>
+      <c r="H24" s="94" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" s="91">
+        <f>I23/I22</f>
+        <v>0.41776937618147447</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B25" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="68">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B23" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="67">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="68">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C25" s="69">
-        <f>SUM(C20:C24)</f>
-        <v>610</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="28" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="36" t="s">
+    <row r="26" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C26" s="69">
+        <f>SUM(C21:C25)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="29" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B30" s="37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B29" s="37" t="s">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B31" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B30" s="38" t="s">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B32" s="39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B31" s="39" t="s">
+    <row r="33" spans="2:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="40" t="s">
-        <v>41</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2677,77 +3233,77 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
-    <col min="3" max="3" width="41.73046875" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.19921875" customWidth="1"/>
+    <col min="3" max="3" width="75.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.86328125" style="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.73046875" customWidth="1"/>
+    <col min="10" max="10" width="15.796875" customWidth="1"/>
     <col min="11" max="11" width="131" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="100"/>
-    </row>
-    <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
+    </row>
+    <row r="3" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="J3" s="48">
         <f>'Cost Summary'!C3</f>
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
       <c r="C4" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -2763,289 +3319,295 @@
       </c>
       <c r="J4" s="19">
         <f>I4*J3</f>
-        <v>211.5</v>
+        <v>352.5</v>
       </c>
       <c r="K4" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5">
-        <v>0.79</v>
+        <v>0.19</v>
       </c>
       <c r="H5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" ref="I5:I11" si="0">H5*G5</f>
-        <v>0.79</v>
+        <f t="shared" ref="I5:I10" si="0">H5*G5</f>
+        <v>1.1400000000000001</v>
       </c>
       <c r="J5" s="6">
         <f>I5*J3</f>
-        <v>118.5</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+        <v>285.00000000000006</v>
+      </c>
+      <c r="K5" s="87" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <v>1206</v>
+      </c>
       <c r="G6" s="5">
-        <v>0.19</v>
+        <v>0.01</v>
       </c>
       <c r="H6" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="0"/>
-        <v>1.1400000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="J6" s="6">
         <f>I6*J3</f>
-        <v>171.00000000000003</v>
-      </c>
-      <c r="K6" s="88" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7" s="14"/>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
-        <v>1206</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="H7" s="4">
-        <v>10</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="C7" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33">
+        <v>0.41</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1</v>
+      </c>
+      <c r="I7" s="34">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="6">
+        <v>0.41</v>
+      </c>
+      <c r="J7" s="34">
         <f>I7*J3</f>
-        <v>15</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+        <v>102.5</v>
+      </c>
+      <c r="K7" s="104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B8" s="14"/>
-      <c r="C8" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33">
-        <v>0.44</v>
-      </c>
-      <c r="H8" s="32">
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="6">
         <f t="shared" si="0"/>
-        <v>0.44</v>
-      </c>
-      <c r="J8" s="34">
+        <v>0.13</v>
+      </c>
+      <c r="J8" s="6">
         <f>I8*J3</f>
-        <v>66</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+        <v>32.5</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>603</v>
+      </c>
       <c r="G9" s="5">
-        <v>0.13</v>
+        <v>0.01</v>
       </c>
       <c r="H9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="0"/>
-        <v>0.13</v>
+        <v>0.02</v>
       </c>
       <c r="J9" s="6">
         <f>I9*J3</f>
-        <v>19.5</v>
+        <v>5</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B10" s="14"/>
-      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="15"/>
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9">
         <v>603</v>
       </c>
-      <c r="G10" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="J10" s="6">
-        <f>I10*J3</f>
-        <v>3</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="15"/>
-      <c r="C11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9">
-        <v>603</v>
-      </c>
-      <c r="G11" s="10">
+      <c r="G10" s="10">
         <v>0.24</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H10" s="11">
         <v>1</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I10" s="12">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="J11" s="12">
-        <f>I11*J3</f>
-        <v>36</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="J10" s="12">
+        <f>I10*J3</f>
+        <v>60</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H11">
+        <f>SUM(H4:H10)</f>
+        <v>22</v>
+      </c>
+      <c r="I11" s="45">
+        <f>SUM(I4:I10)</f>
+        <v>3.45</v>
+      </c>
+      <c r="J11" s="46">
+        <f>SUM(J3:J10)</f>
+        <v>1112.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="116" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="118"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I12" s="45">
-        <f>SUM(I4:I11)</f>
-        <v>4.2700000000000005</v>
-      </c>
-      <c r="J12" s="46">
-        <f>SUM(J3:J11)</f>
-        <v>790.5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="100"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B15" s="25" t="s">
+      <c r="C14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="E14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="F14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="G14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="H14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="I14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="49">
+      <c r="J14" s="49">
         <f>J3</f>
-        <v>150</v>
-      </c>
-      <c r="K15" s="28"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B16" s="14"/>
+        <v>250</v>
+      </c>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="14"/>
+      <c r="C15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6">
+        <f>H15*G15</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J15" s="6">
+        <f>I15*J14</f>
+        <v>140</v>
+      </c>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="14"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.6</v>
       </c>
       <c r="H16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="6">
         <f>H16*G16</f>
-        <v>0.56000000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="J16" s="6">
-        <f>I16*J15</f>
-        <v>84.000000000000014</v>
-      </c>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <f>I16*J3</f>
+        <v>150</v>
+      </c>
+      <c r="K16" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="15"/>
       <c r="C17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -3061,33 +3623,34 @@
         <v>0.86</v>
       </c>
       <c r="J17" s="12">
-        <f>I17*J15</f>
-        <v>129</v>
-      </c>
-      <c r="K17" s="29"/>
-    </row>
-    <row r="18" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <f>I17*J14</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="I18" s="45">
-        <f>SUM(I16:I17)</f>
-        <v>1.42</v>
+        <f>SUM(I15:I17)</f>
+        <v>2.02</v>
       </c>
       <c r="J18" s="47">
-        <f>SUM(J16:J17)</f>
-        <v>213</v>
+        <f>SUM(J15:J17)</f>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B13:K13"/>
     <mergeCell ref="B2:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K11" r:id="rId1" xr:uid="{D6A3A7F7-99EF-4735-9B85-F76458A526A1}"/>
-    <hyperlink ref="K6" r:id="rId2" xr:uid="{69AC4793-AFA7-45EC-9154-F99755E7A340}"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{D6A3A7F7-99EF-4735-9B85-F76458A526A1}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{69AC4793-AFA7-45EC-9154-F99755E7A340}"/>
+    <hyperlink ref="K16" r:id="rId3" xr:uid="{5109247C-C2B0-4A4F-A98F-FC1BF3AB020D}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{847C5AE6-7E2D-45CB-BD02-EFD55D735855}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3095,55 +3658,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4301377-AA15-484C-9B9E-5F5D243282E9}">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="71" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="123.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="123.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="100"/>
+      <c r="B2" s="116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="J3" s="48">
         <f>'Cost Summary'!F3</f>
@@ -3154,7 +3717,7 @@
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
       <c r="C4" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -3180,7 +3743,7 @@
     <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3200,13 +3763,13 @@
         <v>38</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -3226,13 +3789,13 @@
         <v>39</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" s="14"/>
       <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -3254,13 +3817,13 @@
         <v>5</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="14"/>
       <c r="C8" s="32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
@@ -3280,13 +3843,13 @@
         <v>22</v>
       </c>
       <c r="K8" s="35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -3306,13 +3869,13 @@
         <v>6.5</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3334,13 +3897,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="15"/>
       <c r="C11" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -3362,7 +3925,7 @@
         <v>12</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3377,43 +3940,43 @@
     </row>
     <row r="13" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="100"/>
+      <c r="B14" s="116" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="117"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="117"/>
+      <c r="K14" s="118"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="D15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="E15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="F15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="G15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="H15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="I15" s="26" t="s">
         <v>21</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>22</v>
       </c>
       <c r="J15" s="49">
         <f>J3</f>
@@ -3424,10 +3987,10 @@
     <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B16" s="14"/>
       <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -3450,7 +4013,7 @@
     <row r="17" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="15"/>
       <c r="C17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -3499,73 +4062,73 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="123.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="123.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="100"/>
+      <c r="B2" s="116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="J3" s="48">
         <f>'Cost Summary'!I3</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="14"/>
       <c r="C4" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="G4" s="5">
         <v>0.1</v>
@@ -3579,21 +4142,21 @@
       </c>
       <c r="J4" s="6">
         <f>I4*J3</f>
-        <v>10</v>
-      </c>
-      <c r="K4" s="89" t="s">
-        <v>51</v>
+        <v>15</v>
+      </c>
+      <c r="K4" s="88" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="5">
         <v>0.05</v>
@@ -3607,21 +4170,21 @@
       </c>
       <c r="J5" s="6">
         <f>I5*J3</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="15"/>
       <c r="C6" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="10">
         <v>0.01</v>
@@ -3635,10 +4198,10 @@
       </c>
       <c r="J6" s="12">
         <f>I6*J3</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3648,65 +4211,65 @@
       </c>
       <c r="J7" s="53">
         <f>SUM(J4:J6)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="9" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="100"/>
+      <c r="B9" s="116" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="118"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="D10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="E10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="F10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="G10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="H10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="I10" s="26" t="s">
         <v>21</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>22</v>
       </c>
       <c r="J10" s="49">
         <f>J3</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K10" s="28"/>
     </row>
     <row r="11" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="14"/>
       <c r="C11" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="F11" s="65">
         <v>2032</v>
@@ -3723,24 +4286,24 @@
       </c>
       <c r="J11" s="6">
         <f>I11*J10</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="84"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="65"/>
-      <c r="G12" s="85">
+      <c r="G12" s="84">
         <v>0.16</v>
       </c>
-      <c r="H12" s="86">
+      <c r="H12" s="85">
         <v>1</v>
       </c>
       <c r="I12" s="6">
@@ -3749,14 +4312,14 @@
       </c>
       <c r="J12" s="6">
         <f>I12*J10</f>
-        <v>16</v>
-      </c>
-      <c r="K12" s="87"/>
+        <v>24</v>
+      </c>
+      <c r="K12" s="86"/>
     </row>
     <row r="13" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="15"/>
       <c r="C13" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -3773,7 +4336,7 @@
       </c>
       <c r="J13" s="12">
         <f>I13*J10</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="K13" s="29"/>
     </row>
@@ -3785,7 +4348,7 @@
       </c>
       <c r="J14" s="47">
         <f>SUM(J11:J13)</f>
-        <v>41</v>
+        <v>61.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>